<commit_message>
feat: add num of words and num of sentences to first study stats
</commit_message>
<xml_diff>
--- a/excel_stats/statistics_first_metric_prompt.xlsx
+++ b/excel_stats/statistics_first_metric_prompt.xlsx
@@ -2,14 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -25,9 +26,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Calibri"/>
       <b val="1"/>
-      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -47,19 +46,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -72,7 +62,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -435,13 +425,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D100"/>
+  <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.6"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -451,7 +441,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Enhanced Text</t>
+          <t>Simplified Text</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -461,7 +451,27 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Readability Enhanced</t>
+          <t>Readability Simplified</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Words Original</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Words Simplified</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Sentences Original</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Sentences Simplified</t>
         </is>
       </c>
     </row>
@@ -508,6 +518,18 @@
       <c r="D2" t="n">
         <v>10.3034962406015</v>
       </c>
+      <c r="E2" t="n">
+        <v>649</v>
+      </c>
+      <c r="F2" t="n">
+        <v>456</v>
+      </c>
+      <c r="G2" t="n">
+        <v>43</v>
+      </c>
+      <c r="H2" t="n">
+        <v>42</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -531,6 +553,18 @@
       </c>
       <c r="D3" t="n">
         <v>6.61226732267323</v>
+      </c>
+      <c r="E3" t="n">
+        <v>827</v>
+      </c>
+      <c r="F3" t="n">
+        <v>271</v>
+      </c>
+      <c r="G3" t="n">
+        <v>41</v>
+      </c>
+      <c r="H3" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="4">
@@ -559,6 +593,18 @@
       </c>
       <c r="D4" t="n">
         <v>7.924441964285716</v>
+      </c>
+      <c r="E4" t="n">
+        <v>835</v>
+      </c>
+      <c r="F4" t="n">
+        <v>256</v>
+      </c>
+      <c r="G4" t="n">
+        <v>38</v>
+      </c>
+      <c r="H4" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="5">
@@ -590,6 +636,18 @@
       <c r="D5" t="n">
         <v>13.02307390451276</v>
       </c>
+      <c r="E5" t="n">
+        <v>791</v>
+      </c>
+      <c r="F5" t="n">
+        <v>139</v>
+      </c>
+      <c r="G5" t="n">
+        <v>42</v>
+      </c>
+      <c r="H5" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -614,6 +672,18 @@
       <c r="D6" t="n">
         <v>13.46867647058824</v>
       </c>
+      <c r="E6" t="n">
+        <v>554</v>
+      </c>
+      <c r="F6" t="n">
+        <v>272</v>
+      </c>
+      <c r="G6" t="n">
+        <v>30</v>
+      </c>
+      <c r="H6" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -634,6 +704,18 @@
       </c>
       <c r="D7" t="n">
         <v>6.931888111888114</v>
+      </c>
+      <c r="E7" t="n">
+        <v>256</v>
+      </c>
+      <c r="F7" t="n">
+        <v>104</v>
+      </c>
+      <c r="G7" t="n">
+        <v>14</v>
+      </c>
+      <c r="H7" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="8">
@@ -660,6 +742,18 @@
       <c r="D8" t="n">
         <v>13.094</v>
       </c>
+      <c r="E8" t="n">
+        <v>475</v>
+      </c>
+      <c r="F8" t="n">
+        <v>250</v>
+      </c>
+      <c r="G8" t="n">
+        <v>26</v>
+      </c>
+      <c r="H8" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -678,6 +772,18 @@
       </c>
       <c r="D9" t="n">
         <v>14.78396551724138</v>
+      </c>
+      <c r="E9" t="n">
+        <v>191</v>
+      </c>
+      <c r="F9" t="n">
+        <v>116</v>
+      </c>
+      <c r="G9" t="n">
+        <v>10</v>
+      </c>
+      <c r="H9" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="10">
@@ -709,6 +815,18 @@
       <c r="D10" t="n">
         <v>11.83270484581498</v>
       </c>
+      <c r="E10" t="n">
+        <v>628</v>
+      </c>
+      <c r="F10" t="n">
+        <v>227</v>
+      </c>
+      <c r="G10" t="n">
+        <v>32</v>
+      </c>
+      <c r="H10" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -728,6 +846,18 @@
       <c r="D11" t="n">
         <v>8.545454545454547</v>
       </c>
+      <c r="E11" t="n">
+        <v>151</v>
+      </c>
+      <c r="F11" t="n">
+        <v>110</v>
+      </c>
+      <c r="G11" t="n">
+        <v>9</v>
+      </c>
+      <c r="H11" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -746,6 +876,18 @@
       </c>
       <c r="D12" t="n">
         <v>11.80226779026217</v>
+      </c>
+      <c r="E12" t="n">
+        <v>780</v>
+      </c>
+      <c r="F12" t="n">
+        <v>267</v>
+      </c>
+      <c r="G12" t="n">
+        <v>40</v>
+      </c>
+      <c r="H12" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="13">
@@ -771,6 +913,18 @@
       <c r="D13" t="n">
         <v>14.97469387755102</v>
       </c>
+      <c r="E13" t="n">
+        <v>552</v>
+      </c>
+      <c r="F13" t="n">
+        <v>245</v>
+      </c>
+      <c r="G13" t="n">
+        <v>29</v>
+      </c>
+      <c r="H13" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -794,6 +948,18 @@
       <c r="D14" t="n">
         <v>13.34</v>
       </c>
+      <c r="E14" t="n">
+        <v>514</v>
+      </c>
+      <c r="F14" t="n">
+        <v>205</v>
+      </c>
+      <c r="G14" t="n">
+        <v>28</v>
+      </c>
+      <c r="H14" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -813,6 +979,18 @@
       <c r="D15" t="n">
         <v>6.706666666666667</v>
       </c>
+      <c r="E15" t="n">
+        <v>254</v>
+      </c>
+      <c r="F15" t="n">
+        <v>120</v>
+      </c>
+      <c r="G15" t="n">
+        <v>16</v>
+      </c>
+      <c r="H15" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -831,6 +1009,18 @@
       </c>
       <c r="D16" t="n">
         <v>12.97369230769231</v>
+      </c>
+      <c r="E16" t="n">
+        <v>87</v>
+      </c>
+      <c r="F16" t="n">
+        <v>52</v>
+      </c>
+      <c r="G16" t="n">
+        <v>6</v>
+      </c>
+      <c r="H16" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="17">
@@ -854,6 +1044,18 @@
       </c>
       <c r="D17" t="n">
         <v>8.648253205128206</v>
+      </c>
+      <c r="E17" t="n">
+        <v>626</v>
+      </c>
+      <c r="F17" t="n">
+        <v>195</v>
+      </c>
+      <c r="G17" t="n">
+        <v>42</v>
+      </c>
+      <c r="H17" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="18">
@@ -889,6 +1091,18 @@
       <c r="D18" t="n">
         <v>12.3827380952381</v>
       </c>
+      <c r="E18" t="n">
+        <v>849</v>
+      </c>
+      <c r="F18" t="n">
+        <v>336</v>
+      </c>
+      <c r="G18" t="n">
+        <v>41</v>
+      </c>
+      <c r="H18" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -918,6 +1132,18 @@
       <c r="D19" t="n">
         <v>10.23381263616558</v>
       </c>
+      <c r="E19" t="n">
+        <v>503</v>
+      </c>
+      <c r="F19" t="n">
+        <v>216</v>
+      </c>
+      <c r="G19" t="n">
+        <v>30</v>
+      </c>
+      <c r="H19" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -940,6 +1166,18 @@
       </c>
       <c r="D20" t="n">
         <v>13.89320754716982</v>
+      </c>
+      <c r="E20" t="n">
+        <v>292</v>
+      </c>
+      <c r="F20" t="n">
+        <v>159</v>
+      </c>
+      <c r="G20" t="n">
+        <v>13</v>
+      </c>
+      <c r="H20" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="21">
@@ -965,6 +1203,18 @@
       </c>
       <c r="D21" t="n">
         <v>10.30213705583757</v>
+      </c>
+      <c r="E21" t="n">
+        <v>297</v>
+      </c>
+      <c r="F21" t="n">
+        <v>197</v>
+      </c>
+      <c r="G21" t="n">
+        <v>14</v>
+      </c>
+      <c r="H21" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="22">
@@ -992,6 +1242,18 @@
       </c>
       <c r="D22" t="n">
         <v>12.29547511312217</v>
+      </c>
+      <c r="E22" t="n">
+        <v>507</v>
+      </c>
+      <c r="F22" t="n">
+        <v>260</v>
+      </c>
+      <c r="G22" t="n">
+        <v>22</v>
+      </c>
+      <c r="H22" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="23">
@@ -1049,6 +1311,18 @@
       <c r="D23" t="n">
         <v>13.64263440860215</v>
       </c>
+      <c r="E23" t="n">
+        <v>549</v>
+      </c>
+      <c r="F23" t="n">
+        <v>372</v>
+      </c>
+      <c r="G23" t="n">
+        <v>30</v>
+      </c>
+      <c r="H23" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1071,6 +1345,18 @@
       </c>
       <c r="D24" t="n">
         <v>9.739264572636667</v>
+      </c>
+      <c r="E24" t="n">
+        <v>580</v>
+      </c>
+      <c r="F24" t="n">
+        <v>301</v>
+      </c>
+      <c r="G24" t="n">
+        <v>23</v>
+      </c>
+      <c r="H24" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="25">
@@ -1097,6 +1383,18 @@
       <c r="D25" t="n">
         <v>15.25699346405229</v>
       </c>
+      <c r="E25" t="n">
+        <v>507</v>
+      </c>
+      <c r="F25" t="n">
+        <v>306</v>
+      </c>
+      <c r="G25" t="n">
+        <v>22</v>
+      </c>
+      <c r="H25" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1115,6 +1413,18 @@
       </c>
       <c r="D26" t="n">
         <v>9.709004438807863</v>
+      </c>
+      <c r="E26" t="n">
+        <v>828</v>
+      </c>
+      <c r="F26" t="n">
+        <v>249</v>
+      </c>
+      <c r="G26" t="n">
+        <v>49</v>
+      </c>
+      <c r="H26" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="27">
@@ -1146,6 +1456,18 @@
       <c r="D27" t="n">
         <v>11.99435918367347</v>
       </c>
+      <c r="E27" t="n">
+        <v>791</v>
+      </c>
+      <c r="F27" t="n">
+        <v>294</v>
+      </c>
+      <c r="G27" t="n">
+        <v>39</v>
+      </c>
+      <c r="H27" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1171,6 +1493,18 @@
       <c r="D28" t="n">
         <v>10.64016535433071</v>
       </c>
+      <c r="E28" t="n">
+        <v>265</v>
+      </c>
+      <c r="F28" t="n">
+        <v>127</v>
+      </c>
+      <c r="G28" t="n">
+        <v>17</v>
+      </c>
+      <c r="H28" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1192,6 +1526,18 @@
       <c r="D29" t="n">
         <v>13.03892682926829</v>
       </c>
+      <c r="E29" t="n">
+        <v>455</v>
+      </c>
+      <c r="F29" t="n">
+        <v>328</v>
+      </c>
+      <c r="G29" t="n">
+        <v>23</v>
+      </c>
+      <c r="H29" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1211,6 +1557,18 @@
       <c r="D30" t="n">
         <v>14.34930827067669</v>
       </c>
+      <c r="E30" t="n">
+        <v>402</v>
+      </c>
+      <c r="F30" t="n">
+        <v>266</v>
+      </c>
+      <c r="G30" t="n">
+        <v>15</v>
+      </c>
+      <c r="H30" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1229,6 +1587,18 @@
       </c>
       <c r="D31" t="n">
         <v>11.87714285714286</v>
+      </c>
+      <c r="E31" t="n">
+        <v>95</v>
+      </c>
+      <c r="F31" t="n">
+        <v>80</v>
+      </c>
+      <c r="G31" t="n">
+        <v>8</v>
+      </c>
+      <c r="H31" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="32">
@@ -1270,6 +1640,18 @@
       <c r="D32" t="n">
         <v>10.20202425876011</v>
       </c>
+      <c r="E32" t="n">
+        <v>854</v>
+      </c>
+      <c r="F32" t="n">
+        <v>424</v>
+      </c>
+      <c r="G32" t="n">
+        <v>41</v>
+      </c>
+      <c r="H32" t="n">
+        <v>35</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1288,6 +1670,18 @@
       </c>
       <c r="D33" t="n">
         <v>11.983125</v>
+      </c>
+      <c r="E33" t="n">
+        <v>283</v>
+      </c>
+      <c r="F33" t="n">
+        <v>163</v>
+      </c>
+      <c r="G33" t="n">
+        <v>18</v>
+      </c>
+      <c r="H33" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="34">
@@ -1312,25 +1706,47 @@
       <c r="D34" t="n">
         <v>10.15734693877551</v>
       </c>
+      <c r="E34" t="n">
+        <v>467</v>
+      </c>
+      <c r="F34" t="n">
+        <v>196</v>
+      </c>
+      <c r="G34" t="n">
+        <v>25</v>
+      </c>
+      <c r="H34" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Corrected text:
-The majority of data produced in the current digital era takes the form of natural ubiquitous signals: audio signals, various biometric data, image features, economic data, etc. These are often viewed as time series and need to be organized and searched in a way that is key to research issues drawing a lot of attention in the last two decades. An important problem in this context is the subsequence matching problem. It is basically formulated as follows: given a query sequence, find the best matching subsequences in a database. Depending on the specific data application, this general problem has many variants, with query sequences of fixed or variable sizes and data-specific definitions for sequence matching requirements such as dynamic time warping, etc. Therefore, the research effort in this area has resulted in many approaches and techniques. The general focus is on specific fragments of a complex problem, leading authors in the field to identify two main problems that limit comparability and collaboration among the potential various approaches: data bias and algorithms often evaluated on heterogeneous datasets that influence experimental results. Efforts to overcome data bias have led to the establishment of common sets of data collections and consequent research in the area. However, the bias in implementation persists, obstructing the straightforward combination of compatible approaches whose interconnection could facilitate efficient analysis. This situation has led us to the conclusion that a unified environment for developing, prototyping, testing, and combining subsequence matching approaches is needed. In this paper, we propose a generic subsequence matching framework (SMF). Namely, techniques for subsequence matching identify several common subproblems that approaches deal with in various ways (section X); we target to describe the implementation of the framework (section Y). The power of SMF is demonstrated in the elegant realization of several variants of fundamental subsequence matching algorithms; subsequence matching can be simply implemented with the aid of the framework (section Z). The paper concludes in section Z with future directions covering possible performance boosts enabled by the straightforward cooperation of the framework with advanced distance-based indexing and searching technologies.</t>
+          <t>The majority of data produced in the current digital era takes the form of natural ubiquitous signals: audio signals, various biometric data, image features, economic data, etc. These are often viewed as time series and need to be organized and searched in a way that is key to research issues drawing a lot of attention in the last two decades. An important problem in this context is the subsequence matching problem. It is basically formulated as follows: given a query sequence, find the best matching subsequences in a database. Depending on the specific data application, this general problem has many variants, with query sequences of fixed or variable sizes and data-specific definitions for sequence matching requirements such as dynamic time warping, etc. Therefore, the research effort in this area has resulted in many approaches and techniques. The general focus is on specific fragments of a complex problem, leading authors in the field to identify two main problems that limit comparability and collaboration among the potential various approaches: data bias and algorithms often evaluated on heterogeneous datasets that influence experimental results. Efforts to overcome data bias have led to the establishment of common sets of data collections and consequent research in the area. However, the bias in implementation persists, obstructing the straightforward combination of compatible approaches whose interconnection could facilitate efficient analysis. This situation has led us to the conclusion that a unified environment for developing, prototyping, testing, and combining subsequence matching approaches is needed. In this paper, we propose a generic subsequence matching framework (SMF). Namely, techniques for subsequence matching identify several common subproblems that approaches deal with in various ways (section X); we target to describe the implementation of the framework (section Y). The power of SMF is demonstrated in the elegant realization of several variants of fundamental subsequence matching algorithms; subsequence matching can be simply implemented with the aid of the framework (section Z). The paper concludes in section Z with future directions covering possible performance boosts enabled by the straightforward cooperation of the framework with advanced distance-based indexing and searching technologies.</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Rewritten text:
-In today's digital age, most data comes in the form of common signals like sound, body data, pictures, money information, etc. These signals are often seen as time series and need to be organized and searched in ways crucial for research topics that have been getting a lot of attention recently. A key issue here is the problem of finding matching parts within sequences. To put it simply, the task is to locate the most similar parts to a given query sequence within a database. Depending on the particular data used, this basic problem has many versions, with queries of set or changing sizes and specific ways to define matching requirements for sequences like dynamic time warping. The work in this field has led to various methods and tools being developed. The main focus is on solving smaller parts of a complex issue, which has made experts in the field realize two main issues hindering comparison and cooperation between different methods: biased data and algorithms often tested on different datasets that affect the results. Efforts have been made to address data bias by creating shared datasets for research in this area. Yet, bias in implementation remains, making it hard to combine compatible methods that could improve analysis. This has led to the idea that there should be a unified platform for developing, testing, and combining matching methods. In this paper, we introduce a versatile matching framework (SMF). Specifically, the framework breaks down common issues in matching methods (section X) and explains how it can be implemented (section Y). The strength of SMF is shown in how it simplifies the creation of various matching algorithms, making it easy to implement matching with the framework's help (section Z). The paper ends in section Z by discussing future possibilities for boosting performance through the framework's collaboration with advanced distance-based searching technologies.</t>
+          <t>In today's digital age, most data comes in the form of common signals like sound, body data, pictures, money information, etc. These signals are often seen as time series and need to be organized and searched in ways crucial for research topics that have been getting a lot of attention recently. A key issue here is the problem of finding matching parts within sequences. To put it simply, the task is to locate the most similar parts to a given query sequence within a database. Depending on the particular data used, this basic problem has many versions, with queries of set or changing sizes and specific ways to define matching requirements for sequences like dynamic time warping. The work in this field has led to various methods and tools being developed. The main focus is on solving smaller parts of a complex issue, which has made experts in the field realize two main issues hindering comparison and cooperation between different methods: biased data and algorithms often tested on different datasets that affect the results. Efforts have been made to address data bias by creating shared datasets for research in this area. Yet, bias in implementation remains, making it hard to combine compatible methods that could improve analysis. This has led to the idea that there should be a unified platform for developing, testing, and combining matching methods. In this paper, we introduce a versatile matching framework (SMF). Specifically, the framework breaks down common issues in matching methods (section X) and explains how it can be implemented (section Y). The strength of SMF is shown in how it simplifies the creation of various matching algorithms, making it easy to implement matching with the framework's help (section Z). The paper ends in section Z by discussing future possibilities for boosting performance through the framework's collaboration with advanced distance-based searching technologies.</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>16.59675144508671</v>
+        <v>16.54237209302326</v>
       </c>
       <c r="D35" t="n">
-        <v>12.22548387096774</v>
+        <v>12.14851948051949</v>
+      </c>
+      <c r="E35" t="n">
+        <v>344</v>
+      </c>
+      <c r="F35" t="n">
+        <v>308</v>
+      </c>
+      <c r="G35" t="n">
+        <v>15</v>
+      </c>
+      <c r="H35" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="36">
@@ -1350,6 +1766,18 @@
       </c>
       <c r="D36" t="n">
         <v>9.496562500000003</v>
+      </c>
+      <c r="E36" t="n">
+        <v>295</v>
+      </c>
+      <c r="F36" t="n">
+        <v>128</v>
+      </c>
+      <c r="G36" t="n">
+        <v>15</v>
+      </c>
+      <c r="H36" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="37">
@@ -1381,6 +1809,18 @@
       <c r="D37" t="n">
         <v>12.08381609195403</v>
       </c>
+      <c r="E37" t="n">
+        <v>742</v>
+      </c>
+      <c r="F37" t="n">
+        <v>300</v>
+      </c>
+      <c r="G37" t="n">
+        <v>37</v>
+      </c>
+      <c r="H37" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1407,6 +1847,18 @@
       <c r="D38" t="n">
         <v>11.9625</v>
       </c>
+      <c r="E38" t="n">
+        <v>569</v>
+      </c>
+      <c r="F38" t="n">
+        <v>295</v>
+      </c>
+      <c r="G38" t="n">
+        <v>27</v>
+      </c>
+      <c r="H38" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1425,6 +1877,18 @@
       </c>
       <c r="D39" t="n">
         <v>11.2656043956044</v>
+      </c>
+      <c r="E39" t="n">
+        <v>479</v>
+      </c>
+      <c r="F39" t="n">
+        <v>182</v>
+      </c>
+      <c r="G39" t="n">
+        <v>25</v>
+      </c>
+      <c r="H39" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="40">
@@ -1453,6 +1917,18 @@
       <c r="D40" t="n">
         <v>14.41846785225718</v>
       </c>
+      <c r="E40" t="n">
+        <v>515</v>
+      </c>
+      <c r="F40" t="n">
+        <v>387</v>
+      </c>
+      <c r="G40" t="n">
+        <v>24</v>
+      </c>
+      <c r="H40" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1471,6 +1947,18 @@
       </c>
       <c r="D41" t="n">
         <v>11.92062512603347</v>
+      </c>
+      <c r="E41" t="n">
+        <v>736</v>
+      </c>
+      <c r="F41" t="n">
+        <v>261</v>
+      </c>
+      <c r="G41" t="n">
+        <v>42</v>
+      </c>
+      <c r="H41" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="42">
@@ -1503,6 +1991,18 @@
       <c r="D42" t="n">
         <v>13.69285714285715</v>
       </c>
+      <c r="E42" t="n">
+        <v>539</v>
+      </c>
+      <c r="F42" t="n">
+        <v>306</v>
+      </c>
+      <c r="G42" t="n">
+        <v>24</v>
+      </c>
+      <c r="H42" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1533,6 +2033,18 @@
       <c r="D43" t="n">
         <v>14.75495154591601</v>
       </c>
+      <c r="E43" t="n">
+        <v>824</v>
+      </c>
+      <c r="F43" t="n">
+        <v>394</v>
+      </c>
+      <c r="G43" t="n">
+        <v>45</v>
+      </c>
+      <c r="H43" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1553,25 +2065,47 @@
       <c r="D44" t="n">
         <v>9.22538617886179</v>
       </c>
+      <c r="E44" t="n">
+        <v>801</v>
+      </c>
+      <c r="F44" t="n">
+        <v>123</v>
+      </c>
+      <c r="G44" t="n">
+        <v>36</v>
+      </c>
+      <c r="H44" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Corrected text:
-The scientific process aggregates a large number of scientific results. A common scientific consensus on numerical values is presented across scientific papers and collaborative systems like wikis may easily aggregate textual values from multiple sources. However, they are far limited in their ability to apply the numerical analysis required. For example, meta-analysis researchers have discussed the advantages and disadvantages of tools for conducting systematic reviews like "paper and pencil," spreadsheets, RevMan, web-based specialized applications, etc. In 2009, they concluded that "no single data extraction method is best for all systematic reviews circumstances." For example, RevMan from the Archie Cochrane Library provides an elaborate system for keeping track of and analyzing textual and numerical data for meta-analyses. The system could import information from electronic databases or original meta-analyses, Microsoft Excel spreadsheets, and later distribute them to public websites. Compared to an ordinary spreadsheet, a wiki solution provides data entry provenance, collaborative data entry that can be immediately updated and shared in folders, and cloud-based storage systems that would help collaboration. Spreadsheets yield provenance, but online services like Google Docs may lack meta-analytic plotting facilities found in web-based specialized applications for systematic reviews, which may have a high setup cost. Previously, it was explored a simple online meta-analysis system or a "fielded wiki" in connection with personality genetics specifically implemented for scientific areas. The web service lacks generality for types of meta-analytic data, and furthermore, the system relied on PubMed and Brede Wiki to represent bibliographic information. Following Ward Cunningham's quote, "It's the simplest thing that could possibly work," a present simple system allows for mass meta-analysis of numerical data presented in comma-separated values (CSV), a standard MediaWiki-based wiki. Brede Wiki's URL is http://neuro.imm.dtu.dk/wiki.</t>
+          <t>The scientific process aggregates a large number of scientific results. A common scientific consensus on numerical values is presented across scientific papers and collaborative systems like wikis may easily aggregate textual values from multiple sources. However, they are far limited in their ability to apply the numerical analysis required. For example, meta-analysis researchers have discussed the advantages and disadvantages of tools for conducting systematic reviews like "paper and pencil," spreadsheets, RevMan, web-based specialized applications, etc. In 2009, they concluded that "no single data extraction method is best for all systematic reviews circumstances." For example, RevMan from the Archie Cochrane Library provides an elaborate system for keeping track of and analyzing textual and numerical data for meta-analyses. The system could import information from electronic databases or original meta-analyses, Microsoft Excel spreadsheets, and later distribute them to public websites. Compared to an ordinary spreadsheet, a wiki solution provides data entry provenance, collaborative data entry that can be immediately updated and shared in folders, and cloud-based storage systems that would help collaboration. Spreadsheets yield provenance, but online services like Google Docs may lack meta-analytic plotting facilities found in web-based specialized applications for systematic reviews, which may have a high setup cost. Previously, it was explored a simple online meta-analysis system or a "fielded wiki" in connection with personality genetics specifically implemented for scientific areas. The web service lacks generality for types of meta-analytic data, and furthermore, the system relied on PubMed and Brede Wiki to represent bibliographic information. Following Ward Cunningham's quote, "It's the simplest thing that could possibly work," a present simple system allows for mass meta-analysis of numerical data presented in comma-separated values (CSV), a standard MediaWiki-based wiki. Brede Wiki's URL is http://neuro.imm.dtu.dk/wiki.</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Simplified text:
-The scientific process gathers many research findings. Scientists agree on values in papers and wikis. However, these tools struggle with detailed analysis. Meta-analysis experts debate using tools like "paper and pencil," spreadsheets, RevMan, and web tools. They found no one-size-fits-all method. RevMan in 2009 offered a way to manage and analyze data. It could import data from various sources and share it online. Spreadsheets have their benefits but lack some features of specialized web tools. Researchers tried a simple online system for genetics. It was limited and relied on specific databases. A basic system now allows mass data analysis in a standard wiki format. The URL for the wiki is http://neuro.imm.dtu.dk/wiki.</t>
+          <t>The scientific process gathers many research findings. Scientists agree on values in papers and wikis. However, these tools struggle with detailed analysis. Meta-analysis experts debate using tools like "paper and pencil," spreadsheets, RevMan, and web tools. They found no one-size-fits-all method. RevMan in 2009 offered a way to manage and analyze data. It could import data from various sources and share it online. Spreadsheets have their benefits but lack some features of specialized web tools. Researchers tried a simple online system for genetics. It was limited and relied on specific databases. A basic system now allows mass data analysis in a standard wiki format. The URL for the wiki is http://neuro.imm.dtu.dk/wiki.</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>16.14571665285833</v>
+        <v>16.11132665832291</v>
       </c>
       <c r="D45" t="n">
-        <v>8.258180309734513</v>
+        <v>8.164273648648653</v>
+      </c>
+      <c r="E45" t="n">
+        <v>282</v>
+      </c>
+      <c r="F45" t="n">
+        <v>111</v>
+      </c>
+      <c r="G45" t="n">
+        <v>17</v>
+      </c>
+      <c r="H45" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="46">
@@ -1598,6 +2132,18 @@
       <c r="D46" t="n">
         <v>12.14664285714286</v>
       </c>
+      <c r="E46" t="n">
+        <v>539</v>
+      </c>
+      <c r="F46" t="n">
+        <v>350</v>
+      </c>
+      <c r="G46" t="n">
+        <v>29</v>
+      </c>
+      <c r="H46" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1616,6 +2162,18 @@
       </c>
       <c r="D47" t="n">
         <v>13.07962514199167</v>
+      </c>
+      <c r="E47" t="n">
+        <v>804</v>
+      </c>
+      <c r="F47" t="n">
+        <v>278</v>
+      </c>
+      <c r="G47" t="n">
+        <v>44</v>
+      </c>
+      <c r="H47" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="48">
@@ -1643,6 +2201,18 @@
       <c r="D48" t="n">
         <v>14.21618913594146</v>
       </c>
+      <c r="E48" t="n">
+        <v>530</v>
+      </c>
+      <c r="F48" t="n">
+        <v>209</v>
+      </c>
+      <c r="G48" t="n">
+        <v>26</v>
+      </c>
+      <c r="H48" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1670,6 +2240,18 @@
       <c r="D49" t="n">
         <v>10.13734668335419</v>
       </c>
+      <c r="E49" t="n">
+        <v>461</v>
+      </c>
+      <c r="F49" t="n">
+        <v>235</v>
+      </c>
+      <c r="G49" t="n">
+        <v>17</v>
+      </c>
+      <c r="H49" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1697,6 +2279,18 @@
       <c r="D50" t="n">
         <v>15.85142665952891</v>
       </c>
+      <c r="E50" t="n">
+        <v>572</v>
+      </c>
+      <c r="F50" t="n">
+        <v>467</v>
+      </c>
+      <c r="G50" t="n">
+        <v>24</v>
+      </c>
+      <c r="H50" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1722,6 +2316,18 @@
       </c>
       <c r="D51" t="n">
         <v>7.941610808546297</v>
+      </c>
+      <c r="E51" t="n">
+        <v>742</v>
+      </c>
+      <c r="F51" t="n">
+        <v>217</v>
+      </c>
+      <c r="G51" t="n">
+        <v>33</v>
+      </c>
+      <c r="H51" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="52">
@@ -1754,6 +2360,18 @@
       <c r="D52" t="n">
         <v>14.31327237991266</v>
       </c>
+      <c r="E52" t="n">
+        <v>743</v>
+      </c>
+      <c r="F52" t="n">
+        <v>229</v>
+      </c>
+      <c r="G52" t="n">
+        <v>39</v>
+      </c>
+      <c r="H52" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1785,6 +2403,18 @@
       <c r="D53" t="n">
         <v>14.6339455782313</v>
       </c>
+      <c r="E53" t="n">
+        <v>517</v>
+      </c>
+      <c r="F53" t="n">
+        <v>294</v>
+      </c>
+      <c r="G53" t="n">
+        <v>22</v>
+      </c>
+      <c r="H53" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1812,6 +2442,18 @@
       </c>
       <c r="D54" t="n">
         <v>16.01872731023103</v>
+      </c>
+      <c r="E54" t="n">
+        <v>604</v>
+      </c>
+      <c r="F54" t="n">
+        <v>303</v>
+      </c>
+      <c r="G54" t="n">
+        <v>24</v>
+      </c>
+      <c r="H54" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="55">
@@ -1843,6 +2485,18 @@
       <c r="D55" t="n">
         <v>10.58814536340852</v>
       </c>
+      <c r="E55" t="n">
+        <v>840</v>
+      </c>
+      <c r="F55" t="n">
+        <v>228</v>
+      </c>
+      <c r="G55" t="n">
+        <v>34</v>
+      </c>
+      <c r="H55" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1861,6 +2515,18 @@
       </c>
       <c r="D56" t="n">
         <v>10.31195652173913</v>
+      </c>
+      <c r="E56" t="n">
+        <v>575</v>
+      </c>
+      <c r="F56" t="n">
+        <v>345</v>
+      </c>
+      <c r="G56" t="n">
+        <v>31</v>
+      </c>
+      <c r="H56" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="57">
@@ -1885,6 +2551,18 @@
       </c>
       <c r="D57" t="n">
         <v>15.43513513513514</v>
+      </c>
+      <c r="E57" t="n">
+        <v>817</v>
+      </c>
+      <c r="F57" t="n">
+        <v>185</v>
+      </c>
+      <c r="G57" t="n">
+        <v>35</v>
+      </c>
+      <c r="H57" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="58">
@@ -1918,6 +2596,18 @@
       <c r="D58" t="n">
         <v>14.33635241301908</v>
       </c>
+      <c r="E58" t="n">
+        <v>719</v>
+      </c>
+      <c r="F58" t="n">
+        <v>324</v>
+      </c>
+      <c r="G58" t="n">
+        <v>39</v>
+      </c>
+      <c r="H58" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1937,6 +2627,18 @@
       <c r="D59" t="n">
         <v>7.538850574712644</v>
       </c>
+      <c r="E59" t="n">
+        <v>133</v>
+      </c>
+      <c r="F59" t="n">
+        <v>145</v>
+      </c>
+      <c r="G59" t="n">
+        <v>9</v>
+      </c>
+      <c r="H59" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1955,6 +2657,18 @@
       </c>
       <c r="D60" t="n">
         <v>10.82846753246753</v>
+      </c>
+      <c r="E60" t="n">
+        <v>519</v>
+      </c>
+      <c r="F60" t="n">
+        <v>385</v>
+      </c>
+      <c r="G60" t="n">
+        <v>29</v>
+      </c>
+      <c r="H60" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="61">
@@ -1989,6 +2703,18 @@
       <c r="D61" t="n">
         <v>10.96237943791783</v>
       </c>
+      <c r="E61" t="n">
+        <v>768</v>
+      </c>
+      <c r="F61" t="n">
+        <v>497</v>
+      </c>
+      <c r="G61" t="n">
+        <v>101</v>
+      </c>
+      <c r="H61" t="n">
+        <v>31</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2008,6 +2734,18 @@
       <c r="D62" t="n">
         <v>8.213076923076922</v>
       </c>
+      <c r="E62" t="n">
+        <v>47</v>
+      </c>
+      <c r="F62" t="n">
+        <v>26</v>
+      </c>
+      <c r="G62" t="n">
+        <v>3</v>
+      </c>
+      <c r="H62" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2027,6 +2765,18 @@
       <c r="D63" t="n">
         <v>10.67435366739289</v>
       </c>
+      <c r="E63" t="n">
+        <v>769</v>
+      </c>
+      <c r="F63" t="n">
+        <v>405</v>
+      </c>
+      <c r="G63" t="n">
+        <v>52</v>
+      </c>
+      <c r="H63" t="n">
+        <v>34</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2046,6 +2796,18 @@
       <c r="D64" t="n">
         <v>11.85234394904458</v>
       </c>
+      <c r="E64" t="n">
+        <v>599</v>
+      </c>
+      <c r="F64" t="n">
+        <v>314</v>
+      </c>
+      <c r="G64" t="n">
+        <v>26</v>
+      </c>
+      <c r="H64" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2064,6 +2826,18 @@
       </c>
       <c r="D65" t="n">
         <v>13.62747368421053</v>
+      </c>
+      <c r="E65" t="n">
+        <v>462</v>
+      </c>
+      <c r="F65" t="n">
+        <v>228</v>
+      </c>
+      <c r="G65" t="n">
+        <v>20</v>
+      </c>
+      <c r="H65" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="66">
@@ -2090,6 +2864,18 @@
       </c>
       <c r="D66" t="n">
         <v>12.38166666666666</v>
+      </c>
+      <c r="E66" t="n">
+        <v>807</v>
+      </c>
+      <c r="F66" t="n">
+        <v>240</v>
+      </c>
+      <c r="G66" t="n">
+        <v>56</v>
+      </c>
+      <c r="H66" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="67">
@@ -2121,6 +2907,18 @@
       <c r="D67" t="n">
         <v>14.04954455342237</v>
       </c>
+      <c r="E67" t="n">
+        <v>838</v>
+      </c>
+      <c r="F67" t="n">
+        <v>599</v>
+      </c>
+      <c r="G67" t="n">
+        <v>44</v>
+      </c>
+      <c r="H67" t="n">
+        <v>32</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2139,6 +2937,18 @@
       </c>
       <c r="D68" t="n">
         <v>7.457000000000001</v>
+      </c>
+      <c r="E68" t="n">
+        <v>131</v>
+      </c>
+      <c r="F68" t="n">
+        <v>100</v>
+      </c>
+      <c r="G68" t="n">
+        <v>8</v>
+      </c>
+      <c r="H68" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="69">
@@ -2173,6 +2983,18 @@
       <c r="D69" t="n">
         <v>13.77736211487258</v>
       </c>
+      <c r="E69" t="n">
+        <v>796</v>
+      </c>
+      <c r="F69" t="n">
+        <v>239</v>
+      </c>
+      <c r="G69" t="n">
+        <v>47</v>
+      </c>
+      <c r="H69" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2202,6 +3024,18 @@
       <c r="D70" t="n">
         <v>13.27664921465969</v>
       </c>
+      <c r="E70" t="n">
+        <v>808</v>
+      </c>
+      <c r="F70" t="n">
+        <v>382</v>
+      </c>
+      <c r="G70" t="n">
+        <v>39</v>
+      </c>
+      <c r="H70" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2229,6 +3063,18 @@
       <c r="D71" t="n">
         <v>8.230658127208482</v>
       </c>
+      <c r="E71" t="n">
+        <v>591</v>
+      </c>
+      <c r="F71" t="n">
+        <v>283</v>
+      </c>
+      <c r="G71" t="n">
+        <v>30</v>
+      </c>
+      <c r="H71" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2251,6 +3097,18 @@
       </c>
       <c r="D72" t="n">
         <v>10.7848284166165</v>
+      </c>
+      <c r="E72" t="n">
+        <v>587</v>
+      </c>
+      <c r="F72" t="n">
+        <v>453</v>
+      </c>
+      <c r="G72" t="n">
+        <v>39</v>
+      </c>
+      <c r="H72" t="n">
+        <v>33</v>
       </c>
     </row>
     <row r="73">
@@ -2280,6 +3138,18 @@
       <c r="D73" t="n">
         <v>10.81833132771761</v>
       </c>
+      <c r="E73" t="n">
+        <v>730</v>
+      </c>
+      <c r="F73" t="n">
+        <v>277</v>
+      </c>
+      <c r="G73" t="n">
+        <v>41</v>
+      </c>
+      <c r="H73" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2302,6 +3172,18 @@
       </c>
       <c r="D74" t="n">
         <v>12.58923076923077</v>
+      </c>
+      <c r="E74" t="n">
+        <v>330</v>
+      </c>
+      <c r="F74" t="n">
+        <v>195</v>
+      </c>
+      <c r="G74" t="n">
+        <v>15</v>
+      </c>
+      <c r="H74" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="75">
@@ -2330,6 +3212,18 @@
       <c r="D75" t="n">
         <v>11.74842105263158</v>
       </c>
+      <c r="E75" t="n">
+        <v>427</v>
+      </c>
+      <c r="F75" t="n">
+        <v>285</v>
+      </c>
+      <c r="G75" t="n">
+        <v>24</v>
+      </c>
+      <c r="H75" t="n">
+        <v>19</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2348,6 +3242,18 @@
       </c>
       <c r="D76" t="n">
         <v>15.19821428571429</v>
+      </c>
+      <c r="E76" t="n">
+        <v>700</v>
+      </c>
+      <c r="F76" t="n">
+        <v>336</v>
+      </c>
+      <c r="G76" t="n">
+        <v>32</v>
+      </c>
+      <c r="H76" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="77">
@@ -2378,6 +3284,18 @@
       </c>
       <c r="D77" t="n">
         <v>12.62501495016611</v>
+      </c>
+      <c r="E77" t="n">
+        <v>614</v>
+      </c>
+      <c r="F77" t="n">
+        <v>301</v>
+      </c>
+      <c r="G77" t="n">
+        <v>25</v>
+      </c>
+      <c r="H77" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="78">
@@ -2413,6 +3331,18 @@
       <c r="D78" t="n">
         <v>12.15119047619048</v>
       </c>
+      <c r="E78" t="n">
+        <v>826</v>
+      </c>
+      <c r="F78" t="n">
+        <v>378</v>
+      </c>
+      <c r="G78" t="n">
+        <v>45</v>
+      </c>
+      <c r="H78" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -2431,6 +3361,18 @@
       </c>
       <c r="D79" t="n">
         <v>10.5405376344086</v>
+      </c>
+      <c r="E79" t="n">
+        <v>885</v>
+      </c>
+      <c r="F79" t="n">
+        <v>420</v>
+      </c>
+      <c r="G79" t="n">
+        <v>38</v>
+      </c>
+      <c r="H79" t="n">
+        <v>31</v>
       </c>
     </row>
     <row r="80">
@@ -2457,6 +3399,18 @@
       <c r="D80" t="n">
         <v>12.26713513513514</v>
       </c>
+      <c r="E80" t="n">
+        <v>373</v>
+      </c>
+      <c r="F80" t="n">
+        <v>296</v>
+      </c>
+      <c r="G80" t="n">
+        <v>25</v>
+      </c>
+      <c r="H80" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -2482,6 +3436,18 @@
       <c r="D81" t="n">
         <v>11.13611111111112</v>
       </c>
+      <c r="E81" t="n">
+        <v>642</v>
+      </c>
+      <c r="F81" t="n">
+        <v>288</v>
+      </c>
+      <c r="G81" t="n">
+        <v>23</v>
+      </c>
+      <c r="H81" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -2504,6 +3470,18 @@
       <c r="D82" t="n">
         <v>14.47404761904762</v>
       </c>
+      <c r="E82" t="n">
+        <v>517</v>
+      </c>
+      <c r="F82" t="n">
+        <v>177</v>
+      </c>
+      <c r="G82" t="n">
+        <v>23</v>
+      </c>
+      <c r="H82" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -2526,6 +3504,18 @@
       </c>
       <c r="D83" t="n">
         <v>9.751475113122172</v>
+      </c>
+      <c r="E83" t="n">
+        <v>244</v>
+      </c>
+      <c r="F83" t="n">
+        <v>221</v>
+      </c>
+      <c r="G83" t="n">
+        <v>15</v>
+      </c>
+      <c r="H83" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="84">
@@ -2558,6 +3548,18 @@
       <c r="D84" t="n">
         <v>9.436142857142858</v>
       </c>
+      <c r="E84" t="n">
+        <v>800</v>
+      </c>
+      <c r="F84" t="n">
+        <v>413</v>
+      </c>
+      <c r="G84" t="n">
+        <v>58</v>
+      </c>
+      <c r="H84" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -2588,6 +3590,18 @@
       </c>
       <c r="D85" t="n">
         <v>13.4813672795851</v>
+      </c>
+      <c r="E85" t="n">
+        <v>753</v>
+      </c>
+      <c r="F85" t="n">
+        <v>303</v>
+      </c>
+      <c r="G85" t="n">
+        <v>29</v>
+      </c>
+      <c r="H85" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="86">
@@ -2622,6 +3636,18 @@
       <c r="D86" t="n">
         <v>13.58666666666667</v>
       </c>
+      <c r="E86" t="n">
+        <v>620</v>
+      </c>
+      <c r="F86" t="n">
+        <v>177</v>
+      </c>
+      <c r="G86" t="n">
+        <v>38</v>
+      </c>
+      <c r="H86" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -2654,6 +3680,18 @@
       <c r="D87" t="n">
         <v>12.35795073891626</v>
       </c>
+      <c r="E87" t="n">
+        <v>786</v>
+      </c>
+      <c r="F87" t="n">
+        <v>203</v>
+      </c>
+      <c r="G87" t="n">
+        <v>36</v>
+      </c>
+      <c r="H87" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -2683,6 +3721,18 @@
       </c>
       <c r="D88" t="n">
         <v>12.40921052631579</v>
+      </c>
+      <c r="E88" t="n">
+        <v>818</v>
+      </c>
+      <c r="F88" t="n">
+        <v>285</v>
+      </c>
+      <c r="G88" t="n">
+        <v>39</v>
+      </c>
+      <c r="H88" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="89">
@@ -2717,6 +3767,18 @@
       <c r="D89" t="n">
         <v>11.72961436170213</v>
       </c>
+      <c r="E89" t="n">
+        <v>640</v>
+      </c>
+      <c r="F89" t="n">
+        <v>235</v>
+      </c>
+      <c r="G89" t="n">
+        <v>29</v>
+      </c>
+      <c r="H89" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -2747,6 +3809,18 @@
       </c>
       <c r="D90" t="n">
         <v>13.28180929708057</v>
+      </c>
+      <c r="E90" t="n">
+        <v>550</v>
+      </c>
+      <c r="F90" t="n">
+        <v>347</v>
+      </c>
+      <c r="G90" t="n">
+        <v>29</v>
+      </c>
+      <c r="H90" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="91">
@@ -2788,6 +3862,18 @@
       <c r="D91" t="n">
         <v>12.28570689655173</v>
       </c>
+      <c r="E91" t="n">
+        <v>641</v>
+      </c>
+      <c r="F91" t="n">
+        <v>261</v>
+      </c>
+      <c r="G91" t="n">
+        <v>25</v>
+      </c>
+      <c r="H91" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -2806,6 +3892,18 @@
       </c>
       <c r="D92" t="n">
         <v>14.00033434650456</v>
+      </c>
+      <c r="E92" t="n">
+        <v>550</v>
+      </c>
+      <c r="F92" t="n">
+        <v>188</v>
+      </c>
+      <c r="G92" t="n">
+        <v>26</v>
+      </c>
+      <c r="H92" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="93">
@@ -2835,6 +3933,18 @@
       </c>
       <c r="D93" t="n">
         <v>13.45026866515837</v>
+      </c>
+      <c r="E93" t="n">
+        <v>672</v>
+      </c>
+      <c r="F93" t="n">
+        <v>221</v>
+      </c>
+      <c r="G93" t="n">
+        <v>29</v>
+      </c>
+      <c r="H93" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="94">
@@ -2866,6 +3976,18 @@
       </c>
       <c r="D94" t="n">
         <v>13.64412874583796</v>
+      </c>
+      <c r="E94" t="n">
+        <v>819</v>
+      </c>
+      <c r="F94" t="n">
+        <v>265</v>
+      </c>
+      <c r="G94" t="n">
+        <v>41</v>
+      </c>
+      <c r="H94" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="95">
@@ -2898,6 +4020,18 @@
       <c r="D95" t="n">
         <v>12.56130731441048</v>
       </c>
+      <c r="E95" t="n">
+        <v>631</v>
+      </c>
+      <c r="F95" t="n">
+        <v>229</v>
+      </c>
+      <c r="G95" t="n">
+        <v>31</v>
+      </c>
+      <c r="H95" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -2921,6 +4055,18 @@
       <c r="D96" t="n">
         <v>12.89416156670747</v>
       </c>
+      <c r="E96" t="n">
+        <v>555</v>
+      </c>
+      <c r="F96" t="n">
+        <v>258</v>
+      </c>
+      <c r="G96" t="n">
+        <v>25</v>
+      </c>
+      <c r="H96" t="n">
+        <v>19</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -2942,6 +4088,18 @@
       </c>
       <c r="D97" t="n">
         <v>10.91793522267207</v>
+      </c>
+      <c r="E97" t="n">
+        <v>526</v>
+      </c>
+      <c r="F97" t="n">
+        <v>208</v>
+      </c>
+      <c r="G97" t="n">
+        <v>31</v>
+      </c>
+      <c r="H97" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="98">
@@ -2996,6 +4154,18 @@
       <c r="D98" t="n">
         <v>14.07440579710145</v>
       </c>
+      <c r="E98" t="n">
+        <v>768</v>
+      </c>
+      <c r="F98" t="n">
+        <v>276</v>
+      </c>
+      <c r="G98" t="n">
+        <v>39</v>
+      </c>
+      <c r="H98" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -3014,6 +4184,18 @@
       </c>
       <c r="D99" t="n">
         <v>12.06771061930445</v>
+      </c>
+      <c r="E99" t="n">
+        <v>673</v>
+      </c>
+      <c r="F99" t="n">
+        <v>283</v>
+      </c>
+      <c r="G99" t="n">
+        <v>29</v>
+      </c>
+      <c r="H99" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="100">
@@ -3042,6 +4224,18 @@
       <c r="D100" t="n">
         <v>14.80449370552819</v>
       </c>
+      <c r="E100" t="n">
+        <v>821</v>
+      </c>
+      <c r="F100" t="n">
+        <v>406</v>
+      </c>
+      <c r="G100" t="n">
+        <v>53</v>
+      </c>
+      <c r="H100" t="n">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>